<commit_message>
Changeset requested June 2023
</commit_message>
<xml_diff>
--- a/xlsx/studies.xlsx
+++ b/xlsx/studies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26611"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\john\workspace\catalogueMentalHealth\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emckclac-my.sharepoint.com/personal/k1780970_kcl_ac_uk/Documents/1. Catalogue + work documents/1. Catalogue shared files/1. Catalogue/2. Catalogue study updates/Resource folders/cmhm_20May22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1A74F44-6173-4ACD-AFA9-35C837C915EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="634" documentId="13_ncr:1_{6F82A259-41A7-4DF6-B3CE-4CB00C898517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DAA5005-9160-458A-A748-811A5BE69EF2}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="3585" windowWidth="23145" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study details" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="826">
   <si>
     <t>Code</t>
   </si>
@@ -841,7 +841,7 @@
     <t>&lt;a href="https://borninbradford.nhs.uk/what-we-do/pregnancy-early-years/better-start/"&gt;borninbradford.nhs.uk/what-we-do/pregnancy-early-years/better-start&lt;/a&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The BiBBS study aims to recruit 5000 babies, their mothers and their mothers’ partners over 5 years from January 2016-December 2020 from the three BSB areas. The BSB areas are very ethnically diverse, have higher rates of mortality and  morbidity, infant mortality, obesity and poor oral health compared with Bradford district and England. All pregnant women living in BSB areas who are registered to give birth at Bradford Teaching Hospitals NHS Foundation Trust (BTHFT) will be eligible for recruitment. The BTHFT is the only maternity unit covering this area. All babies born to women who have consented to participate in the cohort study will be included in the cohort. The partners of the women who have consented to take part will also be invited to participate. 
+    <t xml:space="preserve">The BiBBS study's sample size is aimed to be 5000 pregnancies and children born of these pregnancies, with recruitment ongoing from January 2016-2024 from the three BSB areas. The BSB areas are very ethnically diverse, have higher rates of mortality and  morbidity, infant mortality, obesity and poor oral health compared with Bradford district and England. All pregnant women living in BSB areas who are registered to give birth at Bradford Teaching Hospitals NHS Foundation Trust (BTHFT) will be eligible for recruitment. The BTHFT is the only maternity unit covering this area. All babies born to women who have consented to participate in the cohort study will be included in the cohort. The partners of the women who have consented to take part will also be invited to participate. 
 &lt;br&gt;&lt;br&gt;
 A system has been developed to flag all women living in the BSB areas on the electronic maternity system. When women attend their first appointment (around 10–12 weeks gestation), the BSB flag will prompt midwives to provide women with information on BSB and the BiBBS cohort study and obtain verbal assent to data sharing with the BiBBS research team. Researchers will identify eligible women who have provided assent to data sharing, and will approach women during the GTT clinic or other appointment to invite them to participate in the cohort. </t>
   </si>
@@ -1409,7 +1409,7 @@
     <t>1994-5</t>
   </si>
   <si>
-    <t xml:space="preserve">Project proposal - see data access guidance &lt;a href="https://sites.google.com/site/moffittcaspiprojects/"&gt;sites.google.com/site/moffittcaspiprojects&lt;/a&gt; </t>
+    <t xml:space="preserve">Project proposal - see data access guidance &lt;a href="https://sites.duke.edu/moffittcaspiprojects/data-use-guidelines/&lt;/a&gt; </t>
   </si>
   <si>
     <t>Crime and justice data,
@@ -1663,7 +1663,7 @@
   </si>
   <si>
     <t>Project proposal - contact study team &lt;br&gt;
-&lt;a href="https://www.ed.ac.uk/generation-scotland/using-resources/access-to-resources/access-process"&gt;ed.ac.uk/generation-scotland/using-resources/access-to-resources/access-process&lt;/a&gt;</t>
+&lt;a href="https://www.ed.ac.uk/generation-scotland/for-researchers/access"&gt;ed.ac.uk/generation-scotland/for-researchers/access&lt;/a&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Cohort Profile: Generation Scotland: Scottish Family Health Study (GS:SFHS). The study, its participants and their potential for genetic research on health and illness. &lt;br&gt;
@@ -1867,7 +1867,7 @@
     <t>The Hertfordshire Cohort Study (HCS) is a nationally unique study of 3,000 men and women born over 1931-1939 and still resident in the English county of Hertfordshire during the 1990s. The principal objective of the study is to evaluate the relationship between prenatal and early postnatal growth, genetic influences, adult lifestyle and the risk of common age-related disorders such as osteoporosis, osteoarthritis, sarcopenia, type 2 diabetes and cardiovascular disease. The HCS has been a key source of evidence for life course influences on health and disease in later life.</t>
   </si>
   <si>
-    <t>MRC Lifecourse Epidemiology Unit, University of Southampton</t>
+    <t>MRC Lifecourse Epidemiology Centre, University of Southampton</t>
   </si>
   <si>
     <t>&lt;a href="https://www.mrc.soton.ac.uk/herts/"&gt;mrc.soton.ac.uk/herts&lt;/a&gt;</t>
@@ -1884,14 +1884,14 @@
   </si>
   <si>
     <t>42,974 births (Birth records)&lt;br&gt;
-3,225 (HCS1)</t>
-  </si>
-  <si>
-    <t>3,225 (HCS1)</t>
+3,225 (HCS Baseline)</t>
+  </si>
+  <si>
+    <t>3,225 (HCS Baseline)</t>
   </si>
   <si>
     <t>Birth records: birth&lt;br&gt;
-HCS: 59-67 years</t>
+59-73 years at HCS Baseline (1998-2004)</t>
   </si>
   <si>
     <t>1931-39</t>
@@ -1902,7 +1902,11 @@
   </si>
   <si>
     <t>Cohort Profile: The Hertfordshire Cohort Study. &lt;br&gt;
-&lt;a href="https://doi.org/10.1093/ije/dyi127"&gt;doi.org/10.1093/ije/dyi127&lt;/a&gt;</t>
+&lt;a href="https://doi.org/10.1093/ije/dyi127"&gt;doi.org/10.1093/ije/dyi127&lt;/a&gt;
+&lt;br&gt;&lt;br&gt;
+Cohort Profile Update: The Hertfordshire Cohort Study: an overview.&lt;br&gt;
+&lt;a
+href="https://doi.org/10.12688%2Ff1000research.17457.1"&gt;doi.org/10.12688%2Ff1000research.17457.1&lt;/a&gt;</t>
   </si>
   <si>
     <t>MRC BHF ARUK ROS Wellcome SOTON</t>
@@ -2020,13 +2024,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t>EUCom ERC MRC NIHR VR</t>
     </r>
     <r>
@@ -2109,7 +2106,7 @@
   <si>
     <t>Defence Analytical Services and Advice (DASA) identified personnel in all branches who deployed on TELIC 1 in the Joint Operational Area (this will include, for example, Iraq, Cyprus and Oman) and those who did not, but were present in the UK Armed Forces on 1 March 2003. These two populations were stratified by service and enlistment type (regular or reserve), the number of personnel sampled in each era stratum was calculated from the proportion of personnel in each TELIC 1 stratum. Because of concerns about the effects of deployment on reservists, reservists were oversampled by a ratio of 2:1. Of the 17,698 individuals identified by DASA, 10,272 consented to participate and returned questionnaires (58.7%), and were included in the study. A comparison of responders and non-responders showed bias due to non-response to be small and that increasing the response rate had little effect on the results; non-response was not influenced by health status (as assessed by objective data on medical downgrading), but was associated with single and enlisted young men.
 &lt;br&gt;&lt;br&gt;
-The cohort was supplemented with two further groups: the first comprised individuals deployed to Afghanistan over a 12-month period from April 2006, and the second included a replenishment sample comprising personnel who joined the military since the initial sample was recruited in 2003.</t>
+The cohort was supplemented with two further groups in 2007: the first comprised individuals deployed to Afghanistan over a 12-month period from April 2006, and the second included a replenishment sample comprising personnel who joined the military since the initial sample was recruited in 2003. A further replenishment sample was added in 2014 comprising personnel who joined the military between 2009 and 2013.</t>
   </si>
   <si>
     <t>1941-1995</t>
@@ -2126,7 +2123,7 @@
 &lt;a href="https://doi.org/10.1192/bjp.2018.175 "&gt;doi.org/10.1192/bjp.2018.175 &lt;/a&gt;</t>
   </si>
   <si>
-    <t>MoD</t>
+    <t>MoD OfVA</t>
   </si>
   <si>
     <t>Covid-19 data collection,
@@ -2277,6 +2274,7 @@
   </si>
   <si>
     <t>Education data,
+Health data,
 Income/tax and benefits</t>
   </si>
   <si>
@@ -2288,7 +2286,9 @@
 &lt;b&gt;&lt;u&gt;Impactful papers using study data&lt;/b&gt;&lt;/u&gt;&lt;br&gt;
 Childhood psychological distress and youth unemployment: Evidence from two British cohort studies. &lt;a href="https://doi.org/10.1016/j.socscimed.2014.11.023"&gt;doi.org/10.1016/j.socscimed.2014.11.023&lt;/a&gt;&lt;br&gt;
 Pre-pandemic mental health and disruptions to healthcare, economic and housing outcomes during the COVID-19 pandemic: evidence from 12 UK longitudinal studies.  &lt;a href="https://doi.org/10.1192/bjp.2021.132"&gt;doi.org/10.1192/bjp.2021.132&lt;/a&gt;&lt;br&gt;
-Common mental disorders prevalence in adolescents: A systematic review and meta-analyses. &lt;a href="https://doi.org/10.1371/journal.pone.0232007"&gt;doi.org/10.1371/journal.pone.0232007&lt;/a&gt;</t>
+Common mental disorders prevalence in adolescents: A systematic review and meta-analyses. &lt;a href="https://doi.org/10.1371/journal.pone.0232007"&gt;doi.org/10.1371/journal.pone.0232007&lt;/a&gt;&lt;br&gt;
+Mental health during lockdown: evidence from four generations. &lt;a
+href="https://cls.ucl.ac.uk/wp-content/uploads/2017/02/Mental-health-during-lockdown-%E2%80%93-initial-findings-from-COVID-19-survey-1.pdf"&gt;cls.ucl.ac.uk/wp-content/uploads/2017/02/Mental-health-during-lockdown-%E2%80%93-initial-findings-from-COVID-19-survey-1.pdf&lt;/a&gt;</t>
   </si>
   <si>
     <t>ESRC DfE</t>
@@ -2353,7 +2353,7 @@
 &lt;b&gt;&lt;u&gt;Impactful papers using study data&lt;/b&gt;&lt;/u&gt;&lt;br&gt;
 The association between adolescent well-being and digital technology use. &lt;a href="https://doi.org/10.1038/s41562-018-0506-1"&gt;doi.org/10.1038/s41562-018-0506-1&lt;/a&gt;&lt;br&gt;
 Economic deprivation, maternal depression, parenting and children's cognitive and emotional development in early childhood 1. &lt;a href="https://doi.org/10.1111/j.1468-4446.2008.00219.x"&gt;doi.org/10.1111/j.1468-4446.2008.00219.x&lt;/a&gt;&lt;br&gt;
-Changes in millennial adolescent mental health and health-related behaviours over 10 years: a population cohort comparison study.  &lt;a href="https://doi.org/10.1093/ije/dyz006"&gt;doi.org/10.1093/ije/dyz006&lt;/a&gt;</t>
+Correlates of mental illness and wellbeing in children: are they the same? Results from the UK Millennium Cohort Study.  &lt;a href="https://doi.org/10.1016/j.jaac.2016.05.019"&gt;doi.org/10.1016/j.jaac.2016.05.019&lt;/a&gt;</t>
   </si>
   <si>
     <t>ESRC DfE DoHSC DfWP DfT HOUK MoJ NIE Scot Welsh ONS Wellcome DHHS NIH&lt;br&gt;
@@ -2487,7 +2487,7 @@
 &lt;a href="https://doi.org/10.1093/ije/dyy065"&gt;doi.org/10.1093/ije/dyy065&lt;/a&gt; </t>
   </si>
   <si>
-    <t>CRUK</t>
+    <t>CRUK MRC</t>
   </si>
   <si>
     <t>Diet and nutrition,
@@ -2620,6 +2620,12 @@
 Social care - need</t>
   </si>
   <si>
+    <t>Linked administrative data,
+Genetic/genomic data,
+Mapping/spatial data,
+Observational/qualitative data</t>
+  </si>
+  <si>
     <t>NICOLA</t>
   </si>
   <si>
@@ -2666,13 +2672,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t>AtlPhil ESRC UKCRC_NI</t>
     </r>
     <r>
@@ -3183,6 +3182,9 @@
     <t>The Southampton Women’s Survey (SWS) is the only birth cohort study in Europe in which mothers were recruited before conception of the child. The SWS aims to assess the influence of maternal dietary, lifestyle, intrauterine, genetic and epigenetic factors on the children’s health and development, and on the health of the mothers themselves. Using this information, the survey can inform the development of interventions to optimize fetal, infant, and childhood growth and development.</t>
   </si>
   <si>
+    <t>MRC Lifecourse Epidemiology Unit, University of Southampton</t>
+  </si>
+  <si>
     <t>&lt;a href="https://www.mrc.soton.ac.uk/sws/"&gt;mrc.soton.ac.uk/sws&lt;/a&gt;</t>
   </si>
   <si>
@@ -3216,13 +3218,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t xml:space="preserve">MRC BHF </t>
     </r>
     <r>
@@ -3715,7 +3710,7 @@
 &lt;br&gt;&lt;br&gt;
 Inclusion criteria for CYP were: had a referral to the GIDS accepted; awaiting first appointment with the service when baseline measures were completed; speak English; live in the UK or the Republic of Ireland. Exclusion criteria for CYP were: aged &gt;14 years at the time their referral to the GIDS was accepted; already attended an appointment at the GIDS before baseline measures were completed; do not provide assent to take part; and do not have parent/caregiver consent. Parents/caregivers of eligible CYP will be asked to provide informed consent in order to participate and must also be proficient in English and live within the UK or the Republic of Ireland. 
 &lt;br&gt;&lt;br&gt;
-The LOGIC-Q sub-sample was comprised of 40 families who took part in the quantitative LOGIC study. The group was purposively sampled to be diverse in relation to assigned sex at birth, current age, social transition status (socially transitioned, partially socially transitioned and no social transition), ethnicity, diagnosis of Autism Spectrum Disorder (ASD), socio-economic status and geographical location. </t>
+The LOGIC-Q sub-sample was comprised of 39 families who took part in the quantitative LOGIC study. The group was purposively sampled to be diverse in relation to assigned sex at birth, current age, social transition status (socially transitioned, partially socially transitioned and no social transition), ethnicity, diagnosis of Autism, socio-economic status and geographical location. </t>
   </si>
   <si>
     <t>3-17 years</t>
@@ -3727,10 +3722,16 @@
     <t>Includes waves of LOGIC-Q qualitative sub-study</t>
   </si>
   <si>
-    <t xml:space="preserve">Longitudinal Outcomes of Gender Identity in Children (LOGIC): protocol for a prospective longitudinal cohort study of children referred to the UK gender identity development service 
-&lt;br&gt;
+    <t xml:space="preserve">Longitudinal Outcomes of Gender Identity in Children (LOGIC): protocol for a prospective longitudinal cohort study of children referred to the UK gender identity development service &lt;br&gt;
 &lt;a href="http://dx.doi.org/10.1136/bmjopen-2020-045628"&gt;dx.doi.org/10.1136/bmjopen-2020-045628
-&lt;/a&gt; </t>
+&lt;/a&gt; &lt;br&gt;&lt;br&gt;
+Longitudinal Outcomes of Gender Identity in Children (LOGIC): a study protocol for a prospective longitudinal qualitative study of the experiences and well-being of families referred to the UK Gender Identity Development Service&lt;br&gt;
+&lt;a href="http://dx.doi.org/10.1136/bmjopen-2020-047875"&gt;dx.doi.org/10.1136/bmjopen-2020-047875
+&lt;/a&gt; &lt;br&gt;&lt;br&gt;
+Thinking Time, Shifting Goalposts and Ticking Time Bombs: Experiences of Waiting on the Gender Identity Development Service Waiting List&lt;br&gt;
+&lt;a href="https://doi.org/10.3390/ijerph192113883"&gt;doi.org/10.3390/ijerph192113883
+&lt;/a&gt; 
+</t>
   </si>
   <si>
     <t xml:space="preserve">Biomarkers, 
@@ -3773,12 +3774,11 @@
 &lt;a href="https://beta.ukdataservice.ac.uk/datacatalogue/studies/study?id=4800&amp;type=Data%20catalogue"&gt;https://beta.ukdataservice.ac.uk/datacatalogue/studies/study?id=4800&amp;type=Data%20catalogue&lt;/a&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Social work records,
+    <t>Social work records,
 Children’s hearing records,
 Police records,
 School records,
-Geographic records,
-</t>
+Geographic records</t>
   </si>
   <si>
     <t xml:space="preserve">Theory and method in the Edinburgh Study of Youth Transitions and Crime. &lt;a href="https://doi.org/10.1093/bjc/43.1.169"&gt;doi.org/10.1093/bjc/43.1.169
@@ -3812,7 +3812,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3867,30 +3867,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="9"/>
       <color rgb="FF444444"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3970,7 +3956,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4024,9 +4010,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4049,7 +4032,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4064,9 +4046,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4086,10 +4065,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4475,21 +4457,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AMJ87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H9" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="V1" sqref="V1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="47" style="32" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="47" style="30" customWidth="1"/>
     <col min="4" max="4" width="41" style="2" customWidth="1"/>
     <col min="5" max="5" width="45.28515625" style="2" customWidth="1"/>
     <col min="6" max="7" width="44" style="2" customWidth="1"/>
@@ -4512,110 +4493,111 @@
     <col min="24" max="24" width="25.28515625" style="4" customWidth="1"/>
     <col min="25" max="25" width="44" style="3" customWidth="1"/>
     <col min="26" max="26" width="24" style="4" customWidth="1"/>
-    <col min="27" max="27" width="43.7109375" style="37" customWidth="1"/>
+    <col min="27" max="27" width="43.7109375" style="34" customWidth="1"/>
     <col min="28" max="34" width="8.85546875" style="5"/>
-    <col min="1024" max="1024" width="9.140625" customWidth="1"/>
+    <col min="35" max="1023" width="8.85546875" style="6"/>
+    <col min="1024" max="1024" width="9.140625" style="6" customWidth="1"/>
+    <col min="1025" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="27" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:1024" s="26" customFormat="1" ht="24" customHeight="1">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="Q1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="R1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="T1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="U1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="24" t="s">
+      <c r="V1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="25" t="s">
+      <c r="W1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="25" t="s">
+      <c r="X1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="24" t="s">
+      <c r="Y1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="25" t="s">
+      <c r="Z1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="35" t="s">
+      <c r="AA1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AMJ1" s="28"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
     </row>
-    <row r="2" spans="1:1024" s="11" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024" s="11" customFormat="1" ht="195" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -4636,7 +4618,7 @@
       <c r="I2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="14" t="s">
         <v>34</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -4683,7 +4665,7 @@
         <v>47</v>
       </c>
       <c r="Z2" s="4"/>
-      <c r="AA2" s="37"/>
+      <c r="AA2" s="34"/>
       <c r="AB2" s="5"/>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
@@ -4691,16 +4673,16 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="5"/>
       <c r="AH2" s="5"/>
-      <c r="AMJ2"/>
+      <c r="AMJ2" s="6"/>
     </row>
-    <row r="3" spans="1:1024" s="14" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1024" s="14" customFormat="1" ht="126.75" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="37" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -4770,7 +4752,7 @@
       <c r="Z3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AA3" s="36"/>
+      <c r="AA3" s="33"/>
       <c r="AB3" s="8"/>
       <c r="AC3" s="8"/>
       <c r="AD3" s="8"/>
@@ -4778,16 +4760,16 @@
       <c r="AF3" s="8"/>
       <c r="AG3" s="8"/>
       <c r="AH3" s="8"/>
-      <c r="AMJ3"/>
+      <c r="AMJ3" s="6"/>
     </row>
-    <row r="4" spans="1:1024" s="14" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1024" s="14" customFormat="1" ht="135.75" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="30" t="s">
         <v>71</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -4839,7 +4821,7 @@
       <c r="T4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U4" s="39" t="s">
+      <c r="U4" s="36" t="s">
         <v>81</v>
       </c>
       <c r="V4" s="3" t="s">
@@ -4857,7 +4839,7 @@
       <c r="Z4" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AA4" s="37"/>
+      <c r="AA4" s="34"/>
       <c r="AB4" s="5"/>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
@@ -4865,16 +4847,16 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="5"/>
       <c r="AH4" s="5"/>
-      <c r="AMJ4"/>
+      <c r="AMJ4" s="6"/>
     </row>
-    <row r="5" spans="1:1024" s="2" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1024" s="2" customFormat="1" ht="110.1" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="30" t="s">
         <v>87</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -4944,7 +4926,7 @@
       <c r="Z5" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="AA5" s="37" t="s">
+      <c r="AA5" s="34" t="s">
         <v>104</v>
       </c>
       <c r="AB5" s="5"/>
@@ -4954,16 +4936,16 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="5"/>
       <c r="AH5" s="5"/>
-      <c r="AMJ5"/>
+      <c r="AMJ5" s="6"/>
     </row>
-    <row r="6" spans="1:1024" s="14" customFormat="1" ht="276" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1024" s="14" customFormat="1" ht="264">
       <c r="A6" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="30" t="s">
         <v>107</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -5033,7 +5015,7 @@
       <c r="Z6" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="AA6" s="37"/>
+      <c r="AA6" s="34"/>
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
       <c r="AD6" s="5"/>
@@ -5041,16 +5023,16 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="5"/>
       <c r="AH6" s="5"/>
-      <c r="AMJ6"/>
+      <c r="AMJ6" s="6"/>
     </row>
-    <row r="7" spans="1:1024" s="16" customFormat="1" ht="131.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1024" s="16" customFormat="1" ht="131.1" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="30" t="s">
         <v>124</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -5118,7 +5100,7 @@
         <v>83</v>
       </c>
       <c r="Z7" s="4"/>
-      <c r="AA7" s="37"/>
+      <c r="AA7" s="34"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
       <c r="AD7" s="5"/>
@@ -5126,16 +5108,16 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="5"/>
       <c r="AH7" s="5"/>
-      <c r="AMJ7"/>
+      <c r="AMJ7" s="6"/>
     </row>
-    <row r="8" spans="1:1024" s="14" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1024" s="14" customFormat="1" ht="120" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="30" t="s">
         <v>137</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -5203,7 +5185,7 @@
       <c r="Z8" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="AA8" s="37"/>
+      <c r="AA8" s="34"/>
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
       <c r="AD8" s="5"/>
@@ -5211,16 +5193,16 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="5"/>
       <c r="AH8" s="5"/>
-      <c r="AMJ8"/>
+      <c r="AMJ8" s="6"/>
     </row>
-    <row r="9" spans="1:1024" s="14" customFormat="1" ht="123.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1024" s="14" customFormat="1" ht="123.95" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="30" t="s">
         <v>153</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -5290,7 +5272,7 @@
       <c r="Z9" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="AA9" s="37"/>
+      <c r="AA9" s="34"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
@@ -5298,16 +5280,16 @@
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
-      <c r="AMJ9"/>
+      <c r="AMJ9" s="6"/>
     </row>
-    <row r="10" spans="1:1024" s="14" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1024" s="14" customFormat="1" ht="96" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="30" t="s">
         <v>169</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -5377,7 +5359,7 @@
       <c r="Z10" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="AA10" s="37"/>
+      <c r="AA10" s="34"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
@@ -5385,16 +5367,16 @@
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
-      <c r="AMJ10"/>
+      <c r="AMJ10" s="6"/>
     </row>
-    <row r="11" spans="1:1024" s="14" customFormat="1" ht="155.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1024" s="14" customFormat="1" ht="155.1" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="30" t="s">
         <v>186</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -5464,7 +5446,7 @@
       <c r="Z11" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AA11" s="37"/>
+      <c r="AA11" s="34"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
@@ -5472,16 +5454,16 @@
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
-      <c r="AMJ11"/>
+      <c r="AMJ11" s="6"/>
     </row>
-    <row r="12" spans="1:1024" s="14" customFormat="1" ht="207.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1024" s="14" customFormat="1" ht="207.95" customHeight="1">
       <c r="A12" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="30" t="s">
         <v>198</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -5551,7 +5533,7 @@
       <c r="Z12" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="AA12" s="37"/>
+      <c r="AA12" s="34"/>
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
       <c r="AD12" s="5"/>
@@ -5559,16 +5541,16 @@
       <c r="AF12" s="5"/>
       <c r="AG12" s="5"/>
       <c r="AH12" s="5"/>
-      <c r="AMJ12"/>
+      <c r="AMJ12" s="6"/>
     </row>
-    <row r="13" spans="1:1024" s="14" customFormat="1" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1024" s="14" customFormat="1" ht="141.94999999999999" customHeight="1">
       <c r="A13" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="30" t="s">
         <v>215</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -5638,7 +5620,7 @@
       <c r="Z13" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="AA13" s="37"/>
+      <c r="AA13" s="34"/>
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
       <c r="AD13" s="5"/>
@@ -5646,16 +5628,16 @@
       <c r="AF13" s="5"/>
       <c r="AG13" s="5"/>
       <c r="AH13" s="5"/>
-      <c r="AMJ13"/>
+      <c r="AMJ13" s="6"/>
     </row>
-    <row r="14" spans="1:1024" s="16" customFormat="1" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1024" s="16" customFormat="1" ht="162.75" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="30" t="s">
         <v>229</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -5725,7 +5707,7 @@
       <c r="Z14" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="AA14" s="37"/>
+      <c r="AA14" s="34"/>
       <c r="AB14" s="5"/>
       <c r="AC14" s="5"/>
       <c r="AD14" s="5"/>
@@ -5733,16 +5715,16 @@
       <c r="AF14" s="5"/>
       <c r="AG14" s="5"/>
       <c r="AH14" s="5"/>
-      <c r="AMJ14"/>
+      <c r="AMJ14" s="6"/>
     </row>
-    <row r="15" spans="1:1024" s="2" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1024" s="2" customFormat="1" ht="129.94999999999999" customHeight="1">
       <c r="A15" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="30" t="s">
         <v>242</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -5811,7 +5793,7 @@
       <c r="Z15" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="AA15" s="37"/>
+      <c r="AA15" s="34"/>
       <c r="AB15" s="5"/>
       <c r="AC15" s="5"/>
       <c r="AD15" s="5"/>
@@ -5819,16 +5801,16 @@
       <c r="AF15" s="5"/>
       <c r="AG15" s="5"/>
       <c r="AH15" s="5"/>
-      <c r="AMJ15"/>
+      <c r="AMJ15" s="6"/>
     </row>
-    <row r="16" spans="1:1024" s="14" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1024" s="14" customFormat="1" ht="87" customHeight="1">
       <c r="A16" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="30" t="s">
         <v>255</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -5898,7 +5880,7 @@
       <c r="Z16" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="AA16" s="37"/>
+      <c r="AA16" s="34"/>
       <c r="AB16" s="5"/>
       <c r="AC16" s="5"/>
       <c r="AD16" s="5"/>
@@ -5906,16 +5888,16 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="5"/>
       <c r="AH16" s="5"/>
-      <c r="AMJ16"/>
+      <c r="AMJ16" s="6"/>
     </row>
-    <row r="17" spans="1:1024" s="14" customFormat="1" ht="183.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1024" s="14" customFormat="1" ht="183.95" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="30" t="s">
         <v>271</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -5983,7 +5965,7 @@
         <v>67</v>
       </c>
       <c r="Z17" s="10"/>
-      <c r="AA17" s="37"/>
+      <c r="AA17" s="34"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
@@ -5991,16 +5973,16 @@
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
-      <c r="AMJ17"/>
+      <c r="AMJ17" s="6"/>
     </row>
-    <row r="18" spans="1:1024" s="14" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1024" s="14" customFormat="1" ht="103.5" customHeight="1">
       <c r="A18" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="31" t="s">
         <v>285</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -6070,7 +6052,7 @@
       <c r="Z18" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="AA18" s="37"/>
+      <c r="AA18" s="34"/>
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
@@ -6078,16 +6060,16 @@
       <c r="AF18" s="2"/>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
-      <c r="AMJ18"/>
+      <c r="AMJ18" s="6"/>
     </row>
-    <row r="19" spans="1:1024" s="14" customFormat="1" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1024" s="14" customFormat="1" ht="140.1" customHeight="1">
       <c r="A19" s="18" t="s">
         <v>298</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="30" t="s">
         <v>300</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -6155,7 +6137,7 @@
         <v>47</v>
       </c>
       <c r="Z19" s="4"/>
-      <c r="AA19" s="37"/>
+      <c r="AA19" s="34"/>
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
       <c r="AD19" s="5"/>
@@ -6163,16 +6145,16 @@
       <c r="AF19" s="5"/>
       <c r="AG19" s="5"/>
       <c r="AH19" s="5"/>
-      <c r="AMJ19"/>
+      <c r="AMJ19" s="6"/>
     </row>
-    <row r="20" spans="1:1024" s="14" customFormat="1" ht="189.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1024" s="14" customFormat="1" ht="189.95" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>314</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="30" t="s">
         <v>315</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -6240,7 +6222,7 @@
       <c r="Z20" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="AA20" s="37"/>
+      <c r="AA20" s="34"/>
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
       <c r="AD20" s="5"/>
@@ -6248,16 +6230,16 @@
       <c r="AF20" s="5"/>
       <c r="AG20" s="5"/>
       <c r="AH20" s="5"/>
-      <c r="AMJ20"/>
+      <c r="AMJ20" s="6"/>
     </row>
-    <row r="21" spans="1:1024" s="14" customFormat="1" ht="233.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1024" s="14" customFormat="1" ht="233.1" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>332</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="30" t="s">
         <v>333</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -6325,7 +6307,7 @@
         <v>47</v>
       </c>
       <c r="Z21" s="4"/>
-      <c r="AA21" s="37"/>
+      <c r="AA21" s="34"/>
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
       <c r="AD21" s="5"/>
@@ -6333,16 +6315,16 @@
       <c r="AF21" s="5"/>
       <c r="AG21" s="5"/>
       <c r="AH21" s="5"/>
-      <c r="AMJ21"/>
+      <c r="AMJ21" s="6"/>
     </row>
-    <row r="22" spans="1:1024" s="6" customFormat="1" ht="198.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1024" ht="198.95" customHeight="1">
       <c r="A22" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="30" t="s">
         <v>347</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -6390,7 +6372,6 @@
       <c r="R22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="S22" s="2"/>
       <c r="T22" s="8" t="s">
         <v>354</v>
       </c>
@@ -6409,25 +6390,15 @@
       <c r="Y22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="37"/>
-      <c r="AB22" s="5"/>
-      <c r="AC22" s="5"/>
-      <c r="AD22" s="5"/>
-      <c r="AE22" s="5"/>
-      <c r="AF22" s="5"/>
-      <c r="AG22" s="5"/>
-      <c r="AH22" s="5"/>
-      <c r="AMJ22"/>
     </row>
-    <row r="23" spans="1:1024" s="6" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1024" ht="153" customHeight="1">
       <c r="A23" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="30" t="s">
         <v>358</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -6448,7 +6419,7 @@
       <c r="I23" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="39" t="s">
         <v>361</v>
       </c>
       <c r="K23" s="9" t="s">
@@ -6475,7 +6446,6 @@
       <c r="R23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="S23" s="2"/>
       <c r="T23" s="2" t="s">
         <v>366</v>
       </c>
@@ -6488,31 +6458,21 @@
       <c r="W23" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="X23" s="4"/>
       <c r="Y23" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="Z23" s="20" t="s">
+      <c r="Z23" s="19" t="s">
         <v>369</v>
       </c>
-      <c r="AA23" s="37"/>
-      <c r="AB23" s="5"/>
-      <c r="AC23" s="5"/>
-      <c r="AD23" s="5"/>
-      <c r="AE23" s="5"/>
-      <c r="AF23" s="5"/>
-      <c r="AG23" s="5"/>
-      <c r="AH23" s="5"/>
-      <c r="AMJ23"/>
     </row>
-    <row r="24" spans="1:1024" s="6" customFormat="1" ht="186.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1024" ht="186.95" customHeight="1">
       <c r="A24" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>371</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="30" t="s">
         <v>372</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -6560,7 +6520,6 @@
       <c r="R24" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="S24" s="2"/>
       <c r="T24" s="2" t="s">
         <v>383</v>
       </c>
@@ -6580,7 +6539,7 @@
       <c r="Z24" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AA24" s="37" t="s">
+      <c r="AA24" s="34" t="s">
         <v>387</v>
       </c>
       <c r="AB24" s="2"/>
@@ -6590,16 +6549,15 @@
       <c r="AF24" s="2"/>
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
-      <c r="AMJ24"/>
     </row>
-    <row r="25" spans="1:1024" s="6" customFormat="1" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1024" ht="216" customHeight="1">
       <c r="A25" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="20" t="s">
         <v>389</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="30" t="s">
         <v>390</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -6669,7 +6627,6 @@
       <c r="Z25" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="AA25" s="37"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
       <c r="AD25" s="2"/>
@@ -6677,16 +6634,15 @@
       <c r="AF25" s="2"/>
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
-      <c r="AMJ25"/>
     </row>
-    <row r="26" spans="1:1024" s="6" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1024" ht="228" customHeight="1">
       <c r="A26" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="20" t="s">
         <v>404</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="30" t="s">
         <v>405</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -6749,31 +6705,21 @@
       <c r="W26" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="X26" s="4"/>
       <c r="Y26" s="3" t="s">
         <v>386</v>
       </c>
       <c r="Z26" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="AA26" s="37"/>
-      <c r="AB26" s="5"/>
-      <c r="AC26" s="5"/>
-      <c r="AD26" s="5"/>
-      <c r="AE26" s="5"/>
-      <c r="AF26" s="5"/>
-      <c r="AG26" s="5"/>
-      <c r="AH26" s="5"/>
-      <c r="AMJ26"/>
     </row>
-    <row r="27" spans="1:1024" s="6" customFormat="1" ht="201.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1024" ht="201.95" customHeight="1">
       <c r="A27" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>412</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="30" t="s">
         <v>413</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -6843,7 +6789,6 @@
       <c r="Z27" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="AA27" s="37"/>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
@@ -6851,16 +6796,15 @@
       <c r="AF27" s="2"/>
       <c r="AG27" s="2"/>
       <c r="AH27" s="2"/>
-      <c r="AMJ27"/>
     </row>
-    <row r="28" spans="1:1024" s="6" customFormat="1" ht="215.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1024" ht="215.1" customHeight="1">
       <c r="A28" s="18" t="s">
         <v>420</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>421</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="30" t="s">
         <v>422</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -6908,7 +6852,6 @@
       <c r="R28" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="S28" s="2"/>
       <c r="T28" s="2" t="s">
         <v>433</v>
       </c>
@@ -6930,24 +6873,15 @@
       <c r="Z28" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AA28" s="37"/>
-      <c r="AB28" s="5"/>
-      <c r="AC28" s="5"/>
-      <c r="AD28" s="5"/>
-      <c r="AE28" s="5"/>
-      <c r="AF28" s="5"/>
-      <c r="AG28" s="5"/>
-      <c r="AH28" s="5"/>
-      <c r="AMJ28"/>
     </row>
-    <row r="29" spans="1:1024" s="6" customFormat="1" ht="221.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1024" ht="221.1" customHeight="1">
       <c r="A29" s="7" t="s">
         <v>436</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="20" t="s">
         <v>437</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="30" t="s">
         <v>438</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -6995,7 +6929,6 @@
       <c r="R29" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="S29" s="2"/>
       <c r="T29" s="2" t="s">
         <v>449</v>
       </c>
@@ -7017,7 +6950,6 @@
       <c r="Z29" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="AA29" s="37"/>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
@@ -7025,16 +6957,15 @@
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
       <c r="AH29" s="2"/>
-      <c r="AMJ29"/>
     </row>
-    <row r="30" spans="1:1024" s="2" customFormat="1" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1024" s="2" customFormat="1" ht="140.1" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="20" t="s">
         <v>453</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="30" t="s">
         <v>454</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -7103,17 +7034,17 @@
       <c r="Z30" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AA30" s="37"/>
-      <c r="AMJ30"/>
+      <c r="AA30" s="34"/>
+      <c r="AMJ30" s="6"/>
     </row>
-    <row r="31" spans="1:1024" s="6" customFormat="1" ht="152.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1024" ht="152.1" customHeight="1">
       <c r="A31" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="30" t="s">
         <v>467</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -7161,7 +7092,6 @@
       <c r="R31" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="S31" s="2"/>
       <c r="T31" s="2" t="s">
         <v>476</v>
       </c>
@@ -7183,24 +7113,15 @@
       <c r="Z31" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="AA31" s="37"/>
-      <c r="AB31" s="5"/>
-      <c r="AC31" s="5"/>
-      <c r="AD31" s="5"/>
-      <c r="AE31" s="5"/>
-      <c r="AF31" s="5"/>
-      <c r="AG31" s="5"/>
-      <c r="AH31" s="5"/>
-      <c r="AMJ31"/>
     </row>
-    <row r="32" spans="1:1024" s="2" customFormat="1" ht="294" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1024" s="2" customFormat="1" ht="294" customHeight="1">
       <c r="A32" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="20" t="s">
         <v>480</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="30" t="s">
         <v>481</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -7272,17 +7193,17 @@
       <c r="Z32" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AA32" s="37"/>
-      <c r="AMJ32"/>
+      <c r="AA32" s="34"/>
+      <c r="AMJ32" s="6"/>
     </row>
-    <row r="33" spans="1:1024" s="6" customFormat="1" ht="204" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" ht="213.75">
       <c r="A33" s="7" t="s">
         <v>494</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="20" t="s">
         <v>495</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="30" t="s">
         <v>496</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -7354,7 +7275,6 @@
       <c r="Z33" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AA33" s="37"/>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
       <c r="AD33" s="2"/>
@@ -7362,16 +7282,15 @@
       <c r="AF33" s="2"/>
       <c r="AG33" s="2"/>
       <c r="AH33" s="2"/>
-      <c r="AMJ33"/>
     </row>
-    <row r="34" spans="1:1024" s="6" customFormat="1" ht="228" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" ht="264">
       <c r="A34" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="20" t="s">
         <v>505</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="30" t="s">
         <v>506</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -7441,7 +7360,6 @@
       <c r="Z34" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="AA34" s="37"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
       <c r="AD34" s="2"/>
@@ -7449,16 +7367,15 @@
       <c r="AF34" s="2"/>
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
-      <c r="AMJ34"/>
     </row>
-    <row r="35" spans="1:1024" s="6" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" ht="301.5">
       <c r="A35" s="7" t="s">
         <v>517</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="20" t="s">
         <v>518</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C35" s="30" t="s">
         <v>519</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -7530,7 +7447,7 @@
       <c r="Z35" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="AA35" s="38" t="s">
+      <c r="AA35" s="35" t="s">
         <v>529</v>
       </c>
       <c r="AB35" s="12"/>
@@ -7540,16 +7457,15 @@
       <c r="AF35" s="12"/>
       <c r="AG35" s="12"/>
       <c r="AH35" s="12"/>
-      <c r="AMJ35"/>
     </row>
-    <row r="36" spans="1:1024" ht="180" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" ht="162.75">
       <c r="A36" s="7" t="s">
         <v>530</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="20" t="s">
         <v>531</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="30" t="s">
         <v>532</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -7613,14 +7529,14 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:1024" ht="168" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" ht="150.75">
       <c r="A37" s="7" t="s">
         <v>545</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="20" t="s">
         <v>546</v>
       </c>
-      <c r="C37" s="32" t="s">
+      <c r="C37" s="30" t="s">
         <v>547</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -7687,7 +7603,7 @@
         <v>550</v>
       </c>
       <c r="Z37" s="10"/>
-      <c r="AA37" s="36"/>
+      <c r="AA37" s="33"/>
       <c r="AB37" s="8"/>
       <c r="AC37" s="8"/>
       <c r="AD37" s="8"/>
@@ -7696,14 +7612,14 @@
       <c r="AG37" s="8"/>
       <c r="AH37" s="8"/>
     </row>
-    <row r="38" spans="1:1024" ht="228" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" ht="213.75">
       <c r="A38" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="28" t="s">
         <v>560</v>
       </c>
-      <c r="C38" s="32" t="s">
+      <c r="C38" s="30" t="s">
         <v>561</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -7773,14 +7689,14 @@
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:1024" ht="264" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" ht="264">
       <c r="A39" s="7" t="s">
         <v>572</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="20" t="s">
         <v>573</v>
       </c>
-      <c r="C39" s="32" t="s">
+      <c r="C39" s="30" t="s">
         <v>574</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -7848,7 +7764,7 @@
         <v>83</v>
       </c>
       <c r="Z39" s="10" t="s">
-        <v>166</v>
+        <v>584</v>
       </c>
       <c r="AB39" s="2"/>
       <c r="AC39" s="2"/>
@@ -7858,24 +7774,24 @@
       <c r="AG39" s="2"/>
       <c r="AH39" s="2"/>
     </row>
-    <row r="40" spans="1:1024" ht="228" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" ht="213.75">
       <c r="A40" s="18" t="s">
-        <v>584</v>
-      </c>
-      <c r="B40" s="21" t="s">
         <v>585</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="B40" s="20" t="s">
         <v>586</v>
       </c>
+      <c r="C40" s="30" t="s">
+        <v>587</v>
+      </c>
       <c r="D40" s="2" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>32</v>
@@ -7887,43 +7803,43 @@
         <v>211</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="K40" s="13">
         <v>8504</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>58</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="O40" s="8" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="Q40" s="2" t="s">
         <v>62</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="V40" s="3" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="W40" s="4" t="s">
         <v>45</v>
@@ -7932,27 +7848,27 @@
         <v>211</v>
       </c>
       <c r="Y40" s="3" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="Z40" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:1024" ht="276" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" ht="288.75">
       <c r="A41" s="18" t="s">
-        <v>601</v>
-      </c>
-      <c r="B41" s="21" t="s">
         <v>602</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="B41" s="20" t="s">
         <v>603</v>
       </c>
+      <c r="C41" s="30" t="s">
+        <v>604</v>
+      </c>
       <c r="D41" s="2" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>74</v>
@@ -7967,13 +7883,13 @@
         <v>211</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="K41" s="13">
         <v>5362</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>58</v>
@@ -7985,7 +7901,7 @@
         <v>1946</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="Q41" s="2" t="s">
         <v>62</v>
@@ -7994,16 +7910,16 @@
         <v>79</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="U41" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V41" s="3" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="W41" s="4" t="s">
         <v>156</v>
@@ -8015,24 +7931,24 @@
         <v>83</v>
       </c>
       <c r="Z41" s="10" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="42" spans="1:1024" ht="204" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:34" ht="200.25">
       <c r="A42" s="7" t="s">
-        <v>613</v>
-      </c>
-      <c r="B42" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="B42" s="20" t="s">
         <v>615</v>
       </c>
+      <c r="C42" s="30" t="s">
+        <v>616</v>
+      </c>
       <c r="D42" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>470</v>
@@ -8044,10 +7960,10 @@
         <v>2014</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="K42" s="13">
         <v>14000</v>
@@ -8062,10 +7978,10 @@
         <v>204</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="Q42" s="2" t="s">
         <v>62</v>
@@ -8074,13 +7990,13 @@
         <v>41</v>
       </c>
       <c r="T42" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="U42" s="2" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="V42" s="3" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="W42" s="4" t="s">
         <v>45</v>
@@ -8095,21 +8011,21 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:1024" ht="192" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:34" ht="200.25">
       <c r="A43" s="7" t="s">
-        <v>625</v>
-      </c>
-      <c r="B43" s="21" t="s">
         <v>626</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="B43" s="20" t="s">
         <v>627</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>628</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>53</v>
@@ -8121,13 +8037,13 @@
         <v>2015</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>190</v>
@@ -8136,13 +8052,13 @@
         <v>58</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="O43" s="8" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="Q43" s="2" t="s">
         <v>62</v>
@@ -8151,16 +8067,16 @@
         <v>41</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="U43" s="2" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="V43" s="3" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="W43" s="10" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="X43" s="10" t="s">
         <v>183</v>
@@ -8179,27 +8095,27 @@
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
     </row>
-    <row r="44" spans="1:1024" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:34" ht="153" customHeight="1">
       <c r="A44" s="18" t="s">
-        <v>639</v>
-      </c>
-      <c r="B44" s="21" t="s">
         <v>640</v>
       </c>
-      <c r="C44" s="32" t="s">
+      <c r="B44" s="20" t="s">
         <v>641</v>
       </c>
+      <c r="C44" s="30" t="s">
+        <v>642</v>
+      </c>
       <c r="D44" s="2" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>53</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="H44" s="8">
         <v>2006</v>
@@ -8208,13 +8124,13 @@
         <v>45</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>58</v>
@@ -8223,10 +8139,10 @@
         <v>460</v>
       </c>
       <c r="O44" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="Q44" s="2" t="s">
         <v>62</v>
@@ -8236,13 +8152,13 @@
       </c>
       <c r="S44" s="5"/>
       <c r="T44" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="U44" s="2" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="V44" s="3" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="W44" s="4" t="s">
         <v>45</v>
@@ -8254,27 +8170,27 @@
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:1024" ht="384" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:34" ht="351.75">
       <c r="A45" s="7" t="s">
-        <v>653</v>
-      </c>
-      <c r="B45" s="21" t="s">
         <v>654</v>
       </c>
-      <c r="C45" s="32" t="s">
+      <c r="B45" s="20" t="s">
         <v>655</v>
       </c>
+      <c r="C45" s="30" t="s">
+        <v>656</v>
+      </c>
       <c r="D45" s="2" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>53</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="H45" s="8">
         <v>1988</v>
@@ -8283,25 +8199,25 @@
         <v>45</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="K45" s="13">
         <v>4858</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>58</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="Q45" s="2" t="s">
         <v>62</v>
@@ -8310,48 +8226,48 @@
         <v>79</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="U45" s="2" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="V45" s="3" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="W45" s="10" t="s">
         <v>45</v>
       </c>
       <c r="X45" s="10" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="Y45" s="3" t="s">
         <v>67</v>
       </c>
       <c r="Z45" s="10" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="46" spans="1:1024" ht="168" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:34" ht="175.5">
       <c r="A46" s="7" t="s">
-        <v>668</v>
-      </c>
-      <c r="B46" s="21" t="s">
         <v>669</v>
       </c>
-      <c r="C46" s="32" t="s">
+      <c r="B46" s="20" t="s">
         <v>670</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>671</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>53</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="H46" s="2">
         <v>2014</v>
@@ -8360,7 +8276,7 @@
         <v>45</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="K46" s="9">
         <v>6616</v>
@@ -8372,28 +8288,28 @@
         <v>58</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="Q46" s="2" t="s">
         <v>62</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>678</v>
-      </c>
-      <c r="U46" s="39" t="s">
         <v>679</v>
       </c>
+      <c r="U46" s="36" t="s">
+        <v>680</v>
+      </c>
       <c r="V46" s="3" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="W46" s="4" t="s">
         <v>45</v>
@@ -8405,21 +8321,21 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:1024" ht="168" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:34" ht="175.5">
       <c r="A47" s="7" t="s">
-        <v>681</v>
-      </c>
-      <c r="B47" s="21" t="s">
         <v>682</v>
       </c>
-      <c r="C47" s="32" t="s">
+      <c r="B47" s="20" t="s">
         <v>683</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>684</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>53</v>
@@ -8434,13 +8350,13 @@
         <v>45</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="M47" s="2" t="s">
         <v>58</v>
@@ -8449,10 +8365,10 @@
         <v>129</v>
       </c>
       <c r="O47" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="Q47" s="2" t="s">
         <v>62</v>
@@ -8461,19 +8377,19 @@
         <v>79</v>
       </c>
       <c r="T47" s="2" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="U47" s="2" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="V47" s="3" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="W47" s="10" t="s">
         <v>45</v>
       </c>
       <c r="X47" s="10" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="Y47" s="3" t="s">
         <v>67</v>
@@ -8489,27 +8405,27 @@
       <c r="AG47" s="2"/>
       <c r="AH47" s="2"/>
     </row>
-    <row r="48" spans="1:1024" ht="300" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:34" ht="264">
       <c r="A48" s="18" t="s">
-        <v>694</v>
-      </c>
-      <c r="B48" s="21" t="s">
         <v>695</v>
       </c>
-      <c r="C48" s="32" t="s">
+      <c r="B48" s="20" t="s">
         <v>696</v>
       </c>
+      <c r="C48" s="30" t="s">
+        <v>697</v>
+      </c>
       <c r="D48" s="2" t="s">
-        <v>423</v>
+        <v>698</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>53</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="H48" s="8">
         <v>1998</v>
@@ -8518,25 +8434,25 @@
         <v>45</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="M48" s="2" t="s">
         <v>58</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="O48" s="8" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="Q48" s="2" t="s">
         <v>62</v>
@@ -8546,13 +8462,13 @@
       </c>
       <c r="S48" s="5"/>
       <c r="T48" s="2" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="U48" s="2" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="V48" s="3" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="W48" s="4" t="s">
         <v>91</v>
@@ -8564,21 +8480,21 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:34" ht="276" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:34" ht="251.25">
       <c r="A49" s="18" t="s">
-        <v>708</v>
-      </c>
-      <c r="B49" s="21" t="s">
-        <v>709</v>
-      </c>
-      <c r="C49" s="32" t="s">
         <v>710</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>711</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>712</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>230</v>
@@ -8593,13 +8509,13 @@
         <v>317</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="M49" s="2" t="s">
         <v>58</v>
@@ -8608,26 +8524,26 @@
         <v>95</v>
       </c>
       <c r="O49" s="8" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>62</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="S49" s="5"/>
       <c r="T49" s="2" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="V49" s="3" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="W49" s="4" t="s">
         <v>328</v>
@@ -8639,21 +8555,21 @@
         <v>330</v>
       </c>
     </row>
-    <row r="50" spans="1:34" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:34" ht="117" customHeight="1">
       <c r="A50" s="18" t="s">
-        <v>721</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>722</v>
-      </c>
-      <c r="C50" s="32" t="s">
         <v>723</v>
       </c>
+      <c r="B50" s="20" t="s">
+        <v>724</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>725</v>
+      </c>
       <c r="D50" s="2" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>470</v>
@@ -8665,28 +8581,28 @@
         <v>1992</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="M50" s="2" t="s">
         <v>58</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="O50" s="2" t="s">
         <v>39</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>62</v>
@@ -8696,16 +8612,16 @@
       </c>
       <c r="S50" s="5"/>
       <c r="T50" s="2" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="U50" s="2" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="V50" s="3" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="W50" s="4" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="Y50" s="3" t="s">
         <v>47</v>
@@ -8713,25 +8629,25 @@
       <c r="Z50" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="AA50" s="37" t="s">
-        <v>736</v>
+      <c r="AA50" s="34" t="s">
+        <v>738</v>
       </c>
     </row>
-    <row r="51" spans="1:34" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:34" ht="78" customHeight="1">
       <c r="A51" s="7" t="s">
-        <v>737</v>
-      </c>
-      <c r="B51" s="21" t="s">
-        <v>738</v>
-      </c>
-      <c r="C51" s="32" t="s">
         <v>739</v>
       </c>
+      <c r="B51" s="20" t="s">
+        <v>740</v>
+      </c>
+      <c r="C51" s="30" t="s">
+        <v>741</v>
+      </c>
       <c r="D51" s="2" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>470</v>
@@ -8740,19 +8656,19 @@
         <v>32</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="M51" s="2" t="s">
         <v>58</v>
@@ -8764,31 +8680,31 @@
         <v>39</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>62</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="T51" s="2" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="U51" s="2" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="V51" s="3" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="W51" s="10" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="X51" s="10" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="Y51" s="3" t="s">
         <v>47</v>
@@ -8804,27 +8720,27 @@
       <c r="AG51" s="2"/>
       <c r="AH51" s="2"/>
     </row>
-    <row r="52" spans="1:34" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:34" ht="87.75" customHeight="1">
       <c r="A52" s="18" t="s">
-        <v>754</v>
-      </c>
-      <c r="B52" s="21" t="s">
-        <v>755</v>
-      </c>
-      <c r="C52" s="32" t="s">
         <v>756</v>
       </c>
+      <c r="B52" s="20" t="s">
+        <v>757</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>758</v>
+      </c>
       <c r="D52" s="2" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>53</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="H52" s="8">
         <v>2007</v>
@@ -8833,10 +8749,10 @@
         <v>91</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="K52" s="13" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>190</v>
@@ -8845,13 +8761,13 @@
         <v>58</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="O52" s="8" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="Q52" s="2" t="s">
         <v>62</v>
@@ -8860,13 +8776,13 @@
         <v>179</v>
       </c>
       <c r="T52" s="2" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="U52" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V52" s="3" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="W52" s="4" t="s">
         <v>91</v>
@@ -8875,24 +8791,24 @@
         <v>67</v>
       </c>
       <c r="Z52" s="10" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
     </row>
-    <row r="53" spans="1:34" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:34" ht="146.25" customHeight="1">
       <c r="A53" s="7" t="s">
-        <v>768</v>
-      </c>
-      <c r="B53" s="21" t="s">
-        <v>769</v>
-      </c>
-      <c r="C53" s="32" t="s">
         <v>770</v>
       </c>
+      <c r="B53" s="20" t="s">
+        <v>771</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>772</v>
+      </c>
       <c r="D53" s="2" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>53</v>
@@ -8904,46 +8820,46 @@
         <v>1985</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="K53" s="13">
         <v>10308</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="M53" s="2" t="s">
         <v>58</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="Q53" s="2" t="s">
         <v>62</v>
       </c>
       <c r="R53" s="2" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="S53" s="2" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="T53" s="2" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="U53" s="2" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="V53" s="3" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="W53" s="4" t="s">
         <v>45</v>
@@ -8958,54 +8874,54 @@
         <v>166</v>
       </c>
     </row>
-    <row r="54" spans="1:34" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:34" ht="113.25" customHeight="1">
       <c r="A54" s="7" t="s">
-        <v>784</v>
-      </c>
-      <c r="B54" s="21" t="s">
-        <v>785</v>
-      </c>
-      <c r="C54" s="32" t="s">
         <v>786</v>
       </c>
+      <c r="B54" s="20" t="s">
+        <v>787</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>788</v>
+      </c>
       <c r="D54" s="2" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>375</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="H54" s="8">
         <v>1986</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="M54" s="2" t="s">
         <v>58</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="Q54" s="2" t="s">
         <v>62</v>
@@ -9014,16 +8930,16 @@
         <v>41</v>
       </c>
       <c r="T54" s="2" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="U54" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V54" s="3" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="W54" s="4" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="Y54" s="3" t="s">
         <v>493</v>
@@ -9032,24 +8948,24 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:34" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:34" ht="389.25">
       <c r="A55" s="7" t="s">
-        <v>798</v>
-      </c>
-      <c r="B55" s="21" t="s">
-        <v>799</v>
-      </c>
-      <c r="C55" s="32" t="s">
         <v>800</v>
       </c>
+      <c r="B55" s="20" t="s">
+        <v>801</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>802</v>
+      </c>
       <c r="D55" s="2" t="s">
-        <v>801</v>
-      </c>
-      <c r="E55" s="41" t="s">
-        <v>802</v>
+        <v>803</v>
+      </c>
+      <c r="E55" s="40" t="s">
+        <v>804</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>32</v>
@@ -9061,25 +8977,25 @@
         <v>45</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="K55" s="2">
         <v>628</v>
       </c>
       <c r="L55" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="M55" s="2" t="s">
         <v>58</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="O55" s="2" t="s">
         <v>39</v>
       </c>
       <c r="P55" s="2" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="Q55" s="2" t="s">
         <v>41</v>
@@ -9087,23 +9003,23 @@
       <c r="R55" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="S55" s="42" t="s">
-        <v>807</v>
+      <c r="S55" s="38" t="s">
+        <v>809</v>
       </c>
       <c r="T55" s="2" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="U55" s="2" t="s">
         <v>181</v>
       </c>
       <c r="V55" s="3" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="W55" s="4" t="s">
         <v>45</v>
       </c>
       <c r="X55" s="4" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="Y55" s="3" t="s">
         <v>47</v>
@@ -9112,27 +9028,27 @@
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="1:34" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:34" ht="389.25">
       <c r="A56" s="7" t="s">
-        <v>811</v>
-      </c>
-      <c r="B56" s="21" t="s">
-        <v>812</v>
-      </c>
-      <c r="C56" s="32" t="s">
         <v>813</v>
       </c>
+      <c r="B56" s="20" t="s">
+        <v>814</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>815</v>
+      </c>
       <c r="D56" s="2" t="s">
-        <v>814</v>
-      </c>
-      <c r="E56" s="41" t="s">
-        <v>815</v>
+        <v>816</v>
+      </c>
+      <c r="E56" s="40" t="s">
+        <v>817</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>375</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="H56" s="2">
         <v>1998</v>
@@ -9141,7 +9057,7 @@
         <v>45</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="K56" s="9">
         <v>4300</v>
@@ -9159,22 +9075,22 @@
         <v>1986</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="Q56" s="2" t="s">
         <v>41</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="T56" s="2" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="U56" s="2" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="V56" s="3" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="W56" s="4" t="s">
         <v>45</v>
@@ -9183,100 +9099,100 @@
         <v>375</v>
       </c>
       <c r="Z56" s="10" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:34">
       <c r="A57" s="7"/>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:34">
       <c r="A58" s="7"/>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:34">
       <c r="A59" s="7"/>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:34">
       <c r="A60" s="7"/>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:34">
       <c r="A61" s="7"/>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:34">
       <c r="A62" s="7"/>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:34">
       <c r="A63" s="7"/>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:34">
       <c r="A64" s="7"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1">
       <c r="A65" s="7"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1">
       <c r="A66" s="7"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1">
       <c r="A67" s="7"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1">
       <c r="A68" s="7"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1">
       <c r="A69" s="7"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1">
       <c r="A70" s="7"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1">
       <c r="A71" s="7"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1">
       <c r="A72" s="7"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1">
       <c r="A73" s="7"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1">
       <c r="A74" s="7"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1">
       <c r="A75" s="7"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1">
       <c r="A76" s="7"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1">
       <c r="A77" s="7"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1">
       <c r="A78" s="7"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1">
       <c r="A79" s="7"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1">
       <c r="A80" s="7"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1">
       <c r="A81" s="7"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1">
       <c r="A82" s="7"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1">
       <c r="A83" s="7"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1">
       <c r="A84" s="7"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1">
       <c r="A85" s="7"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1">
       <c r="A86" s="7"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1">
       <c r="A87" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEP-MD study added - tweak to loading script to account for new studies
</commit_message>
<xml_diff>
--- a/xlsx/studies.xlsx
+++ b/xlsx/studies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emckclac-my.sharepoint.com/personal/k1780970_kcl_ac_uk/Documents/1. Catalogue + work documents/1. Catalogue shared files/1. Catalogue/2. Catalogue study updates/Resource folders/cmhm_20May22/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\john\workspace\catalogueMentalHealth\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="695" documentId="13_ncr:1_{6F82A259-41A7-4DF6-B3CE-4CB00C898517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F3B4F9D-D9B7-4DB9-A9D6-6E04D057A946}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9038C18-B791-4F61-B0DD-3DFE6CFB61C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study details" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="855">
   <si>
     <t>Code</t>
   </si>
@@ -3867,12 +3867,65 @@
     <t>Linked administrative data,
 Mapping/spatial data</t>
   </si>
+  <si>
+    <t>SEP-MD</t>
+  </si>
+  <si>
+    <t>Social and Economic Predictors of the Severe Mental Disorders Study (SEP-MD)</t>
+  </si>
+  <si>
+    <t>The SEP-MD Data Linkage Study is a large linked cohort connecting individual-level records from the 2011 UK Census with de-identified clinical records from the South London &amp; Maudsley Trust, which provides mental health care across South East London, as well as death registrations. The study aims to explore how neighbourhood and individual-level factors are related to mortality, in-patient admissions and long-term worklessness in people with severe mental health conditions. The study will also explore ethnic inequalities to deepen understanding of disparities in outcomes.</t>
+  </si>
+  <si>
+    <t>King's College London</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.kcl.ac.uk/research/the-sep-md-data-linkage-study/"&gt;https://www.kcl.ac.uk/research/the-sep-md-data-linkage-study/&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>South East London</t>
+  </si>
+  <si>
+    <t>Linked cohort</t>
+  </si>
+  <si>
+    <t>The sample consists of de-identified clinical records from South London &amp; Maudsley (SLaM) Trust, one of Europe's largest secondary mental health service providers, which are extracted and accessible through the Clinical Record Interactive Search (CRIS) system. The trust provides mental health care to an ethnically diverse, urbanised location in South East London, with a catchment area of 1.3 million people and only 38.7% of SlaM service users reporting their ethnicity as 'White' in 2020-21. This includes all mental health services provided by the NHS, such as the Improving Access to Psychological Therapies (IAPT) service. These clinical records are linked to individual-level records from the 2011 UK Census, containing information on individual's social and environmental conditions, and death registrations.
+The linked cohort includes 19,808 de-identified records of SLaM service users with a diagnosis of severe mental illness, including Schizophrenia-spectrum disorders, Bipolar affective disorders and non-organic psychoses, linked with available data from the 2011 census. In addition to the linked cohort, an additional sample is available to facilitate further research. For each indivdiual in the SEP-MD cohort, data were matched with 5 controls from the study area who had completed Census questions but did not have a history of severe mental health problems, allowing for examination of the social determinants of onset, course, and outcomes (admissions, worklessness and mortality) in people living with severe mental health conditions.</t>
+  </si>
+  <si>
+    <t>19,808 individuals with a diagnosis of severe mental illness</t>
+  </si>
+  <si>
+    <t>The linked dataset is hosted in an ONS secure setting and is accessible to accredited researchers working on the study, subject to completing an approvals process. Contact Dr Das-Munshi for more information: jayati.das-munshi@kcl.ac.uk</t>
+  </si>
+  <si>
+    <t>Cybulski et al. (2023). Improving our understanding of the social determinants of mental health: A data linkage study of mental health records and the 2011 UK census. &lt;br&gt;
+&lt;a
+href="https://doi.org/10.1101/2023.03.10.23287114"&gt;doi.org/10.1101/2023.03.10.23287114&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>ESRC</t>
+  </si>
+  <si>
+    <t>Cognitive measures,
+Ethnicity and race,
+Housing,
+Language and literacy,
+Neighbourhood,
+Social care - provision,
+Socioeconomic status and deprivation,
+Work and employment</t>
+  </si>
+  <si>
+    <t>Ethnicity and race,
+Patients and clinical cohorts</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3938,8 +3991,27 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF2E2E2E"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3961,6 +4033,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4016,7 +4094,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4133,6 +4211,24 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4520,13 +4616,13 @@
   <dimension ref="A1:AMJ87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AA5" sqref="AA5"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V1" sqref="V1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="V1" sqref="V1"/>
+      <selection pane="bottomRight" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="46.28515625" style="20" customWidth="1"/>
@@ -4560,7 +4656,7 @@
     <col min="1025" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="26" customFormat="1" ht="24" customHeight="1">
+    <row r="1" spans="1:1024" s="26" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4650,7 +4746,7 @@
       <c r="AG1" s="25"/>
       <c r="AH1" s="25"/>
     </row>
-    <row r="2" spans="1:1024" s="11" customFormat="1" ht="195" customHeight="1">
+    <row r="2" spans="1:1024" s="11" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -4735,7 +4831,7 @@
       <c r="AH2" s="5"/>
       <c r="AMJ2" s="6"/>
     </row>
-    <row r="3" spans="1:1024" s="14" customFormat="1" ht="126.75" customHeight="1">
+    <row r="3" spans="1:1024" s="14" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -4822,7 +4918,7 @@
       <c r="AH3" s="8"/>
       <c r="AMJ3" s="6"/>
     </row>
-    <row r="4" spans="1:1024" s="14" customFormat="1" ht="135.75" customHeight="1">
+    <row r="4" spans="1:1024" s="14" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>70</v>
       </c>
@@ -4911,7 +5007,7 @@
       <c r="AH4" s="5"/>
       <c r="AMJ4" s="6"/>
     </row>
-    <row r="5" spans="1:1024" s="2" customFormat="1" ht="110.1" customHeight="1">
+    <row r="5" spans="1:1024" s="2" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>87</v>
       </c>
@@ -5000,7 +5096,7 @@
       <c r="AH5" s="5"/>
       <c r="AMJ5" s="6"/>
     </row>
-    <row r="6" spans="1:1024" s="14" customFormat="1" ht="264">
+    <row r="6" spans="1:1024" s="14" customFormat="1" ht="276" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>107</v>
       </c>
@@ -5087,7 +5183,7 @@
       <c r="AH6" s="5"/>
       <c r="AMJ6" s="6"/>
     </row>
-    <row r="7" spans="1:1024" s="16" customFormat="1" ht="131.1" customHeight="1">
+    <row r="7" spans="1:1024" s="16" customFormat="1" ht="131.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>124</v>
       </c>
@@ -5172,7 +5268,7 @@
       <c r="AH7" s="5"/>
       <c r="AMJ7" s="6"/>
     </row>
-    <row r="8" spans="1:1024" s="14" customFormat="1" ht="120" customHeight="1">
+    <row r="8" spans="1:1024" s="14" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>137</v>
       </c>
@@ -5257,7 +5353,7 @@
       <c r="AH8" s="5"/>
       <c r="AMJ8" s="6"/>
     </row>
-    <row r="9" spans="1:1024" s="14" customFormat="1" ht="123.95" customHeight="1">
+    <row r="9" spans="1:1024" s="14" customFormat="1" ht="123.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>153</v>
       </c>
@@ -5346,7 +5442,7 @@
       <c r="AH9" s="2"/>
       <c r="AMJ9" s="6"/>
     </row>
-    <row r="10" spans="1:1024" s="14" customFormat="1" ht="96" customHeight="1">
+    <row r="10" spans="1:1024" s="14" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>170</v>
       </c>
@@ -5433,7 +5529,7 @@
       <c r="AH10" s="2"/>
       <c r="AMJ10" s="6"/>
     </row>
-    <row r="11" spans="1:1024" s="14" customFormat="1" ht="155.1" customHeight="1">
+    <row r="11" spans="1:1024" s="14" customFormat="1" ht="155.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>187</v>
       </c>
@@ -5520,7 +5616,7 @@
       <c r="AH11" s="2"/>
       <c r="AMJ11" s="6"/>
     </row>
-    <row r="12" spans="1:1024" s="14" customFormat="1" ht="207.95" customHeight="1">
+    <row r="12" spans="1:1024" s="14" customFormat="1" ht="207.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>199</v>
       </c>
@@ -5609,7 +5705,7 @@
       <c r="AH12" s="5"/>
       <c r="AMJ12" s="6"/>
     </row>
-    <row r="13" spans="1:1024" s="14" customFormat="1" ht="141.94999999999999" customHeight="1">
+    <row r="13" spans="1:1024" s="14" customFormat="1" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>217</v>
       </c>
@@ -5696,7 +5792,7 @@
       <c r="AH13" s="5"/>
       <c r="AMJ13" s="6"/>
     </row>
-    <row r="14" spans="1:1024" s="16" customFormat="1" ht="162.75" customHeight="1">
+    <row r="14" spans="1:1024" s="16" customFormat="1" ht="162.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>231</v>
       </c>
@@ -5783,7 +5879,7 @@
       <c r="AH14" s="5"/>
       <c r="AMJ14" s="6"/>
     </row>
-    <row r="15" spans="1:1024" s="2" customFormat="1" ht="129.94999999999999" customHeight="1">
+    <row r="15" spans="1:1024" s="2" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>244</v>
       </c>
@@ -5869,7 +5965,7 @@
       <c r="AH15" s="5"/>
       <c r="AMJ15" s="6"/>
     </row>
-    <row r="16" spans="1:1024" s="14" customFormat="1" ht="87" customHeight="1">
+    <row r="16" spans="1:1024" s="14" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>257</v>
       </c>
@@ -5956,7 +6052,7 @@
       <c r="AH16" s="5"/>
       <c r="AMJ16" s="6"/>
     </row>
-    <row r="17" spans="1:1024" s="14" customFormat="1" ht="183.95" customHeight="1">
+    <row r="17" spans="1:1024" s="14" customFormat="1" ht="183.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>273</v>
       </c>
@@ -6043,7 +6139,7 @@
       <c r="AH17" s="2"/>
       <c r="AMJ17" s="6"/>
     </row>
-    <row r="18" spans="1:1024" s="14" customFormat="1" ht="103.5" customHeight="1">
+    <row r="18" spans="1:1024" s="14" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>288</v>
       </c>
@@ -6132,7 +6228,7 @@
       <c r="AH18" s="2"/>
       <c r="AMJ18" s="6"/>
     </row>
-    <row r="19" spans="1:1024" s="14" customFormat="1" ht="140.1" customHeight="1">
+    <row r="19" spans="1:1024" s="14" customFormat="1" ht="140.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>304</v>
       </c>
@@ -6217,7 +6313,7 @@
       <c r="AH19" s="5"/>
       <c r="AMJ19" s="6"/>
     </row>
-    <row r="20" spans="1:1024" s="14" customFormat="1" ht="189.95" customHeight="1">
+    <row r="20" spans="1:1024" s="14" customFormat="1" ht="189.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>319</v>
       </c>
@@ -6302,7 +6398,7 @@
       <c r="AH20" s="5"/>
       <c r="AMJ20" s="6"/>
     </row>
-    <row r="21" spans="1:1024" s="14" customFormat="1" ht="233.1" customHeight="1">
+    <row r="21" spans="1:1024" s="14" customFormat="1" ht="233.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>337</v>
       </c>
@@ -6387,7 +6483,7 @@
       <c r="AH21" s="5"/>
       <c r="AMJ21" s="6"/>
     </row>
-    <row r="22" spans="1:1024" ht="198.95" customHeight="1">
+    <row r="22" spans="1:1024" ht="198.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>351</v>
       </c>
@@ -6461,7 +6557,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:1024" ht="153" customHeight="1">
+    <row r="23" spans="1:1024" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>363</v>
       </c>
@@ -6535,7 +6631,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="24" spans="1:1024" ht="186.95" customHeight="1">
+    <row r="24" spans="1:1024" ht="186.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>376</v>
       </c>
@@ -6620,7 +6716,7 @@
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
     </row>
-    <row r="25" spans="1:1024" ht="216" customHeight="1">
+    <row r="25" spans="1:1024" ht="216" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>394</v>
       </c>
@@ -6705,7 +6801,7 @@
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
     </row>
-    <row r="26" spans="1:1024" ht="228" customHeight="1">
+    <row r="26" spans="1:1024" ht="228" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>409</v>
       </c>
@@ -6782,7 +6878,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:1024" ht="201.95" customHeight="1">
+    <row r="27" spans="1:1024" ht="201.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>417</v>
       </c>
@@ -6867,7 +6963,7 @@
       <c r="AG27" s="2"/>
       <c r="AH27" s="2"/>
     </row>
-    <row r="28" spans="1:1024" ht="215.1" customHeight="1">
+    <row r="28" spans="1:1024" ht="215.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
         <v>426</v>
       </c>
@@ -6944,7 +7040,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:1024" ht="221.1" customHeight="1">
+    <row r="29" spans="1:1024" ht="221.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>442</v>
       </c>
@@ -7031,7 +7127,7 @@
       <c r="AG29" s="2"/>
       <c r="AH29" s="2"/>
     </row>
-    <row r="30" spans="1:1024" s="2" customFormat="1" ht="140.1" customHeight="1">
+    <row r="30" spans="1:1024" s="2" customFormat="1" ht="140.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>460</v>
       </c>
@@ -7110,7 +7206,7 @@
       <c r="AA30" s="34"/>
       <c r="AMJ30" s="6"/>
     </row>
-    <row r="31" spans="1:1024" ht="152.1" customHeight="1">
+    <row r="31" spans="1:1024" ht="152.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>472</v>
       </c>
@@ -7187,7 +7283,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:1024" s="2" customFormat="1" ht="294" customHeight="1">
+    <row r="32" spans="1:1024" s="2" customFormat="1" ht="294" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>486</v>
       </c>
@@ -7271,7 +7367,7 @@
       </c>
       <c r="AMJ32" s="6"/>
     </row>
-    <row r="33" spans="1:34" ht="213.75">
+    <row r="33" spans="1:34" ht="204" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>502</v>
       </c>
@@ -7361,7 +7457,7 @@
       <c r="AG33" s="2"/>
       <c r="AH33" s="2"/>
     </row>
-    <row r="34" spans="1:34" ht="264">
+    <row r="34" spans="1:34" ht="300" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>513</v>
       </c>
@@ -7449,7 +7545,7 @@
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
     </row>
-    <row r="35" spans="1:34" ht="301.5">
+    <row r="35" spans="1:34" ht="288" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>527</v>
       </c>
@@ -7539,7 +7635,7 @@
       <c r="AG35" s="12"/>
       <c r="AH35" s="12"/>
     </row>
-    <row r="36" spans="1:34" ht="162.75">
+    <row r="36" spans="1:34" ht="180" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>540</v>
       </c>
@@ -7610,7 +7706,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="150.75">
+    <row r="37" spans="1:34" ht="168" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>555</v>
       </c>
@@ -7695,7 +7791,7 @@
       <c r="AG37" s="8"/>
       <c r="AH37" s="8"/>
     </row>
-    <row r="38" spans="1:34" ht="213.75">
+    <row r="38" spans="1:34" ht="228" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>570</v>
       </c>
@@ -7772,7 +7868,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="264">
+    <row r="39" spans="1:34" ht="264" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>583</v>
       </c>
@@ -7860,7 +7956,7 @@
       <c r="AG39" s="2"/>
       <c r="AH39" s="2"/>
     </row>
-    <row r="40" spans="1:34" ht="213.75">
+    <row r="40" spans="1:34" ht="228" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
         <v>597</v>
       </c>
@@ -7940,7 +8036,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="288.75">
+    <row r="41" spans="1:34" ht="276" x14ac:dyDescent="0.2">
       <c r="A41" s="18" t="s">
         <v>614</v>
       </c>
@@ -8023,7 +8119,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="200.25">
+    <row r="42" spans="1:34" ht="204" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>627</v>
       </c>
@@ -8100,7 +8196,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:34" ht="200.25">
+    <row r="43" spans="1:34" ht="192" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>639</v>
       </c>
@@ -8187,7 +8283,7 @@
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
     </row>
-    <row r="44" spans="1:34" ht="153" customHeight="1">
+    <row r="44" spans="1:34" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18" t="s">
         <v>654</v>
       </c>
@@ -8259,7 +8355,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="45" spans="1:34" ht="351.75">
+    <row r="45" spans="1:34" ht="384" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>667</v>
       </c>
@@ -8336,7 +8432,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="46" spans="1:34" ht="175.5">
+    <row r="46" spans="1:34" ht="168" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>682</v>
       </c>
@@ -8410,7 +8506,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="1:34" ht="175.5">
+    <row r="47" spans="1:34" ht="168" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>695</v>
       </c>
@@ -8497,7 +8593,7 @@
       <c r="AG47" s="2"/>
       <c r="AH47" s="2"/>
     </row>
-    <row r="48" spans="1:34" ht="264">
+    <row r="48" spans="1:34" ht="300" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
         <v>709</v>
       </c>
@@ -8572,7 +8668,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:34" ht="251.25">
+    <row r="49" spans="1:34" ht="276" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
         <v>724</v>
       </c>
@@ -8647,7 +8743,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="50" spans="1:34" ht="117" customHeight="1">
+    <row r="50" spans="1:34" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
         <v>737</v>
       </c>
@@ -8725,7 +8821,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="51" spans="1:34" ht="78" customHeight="1">
+    <row r="51" spans="1:34" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>753</v>
       </c>
@@ -8815,7 +8911,7 @@
       <c r="AG51" s="2"/>
       <c r="AH51" s="2"/>
     </row>
-    <row r="52" spans="1:34" ht="87.75" customHeight="1">
+    <row r="52" spans="1:34" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
         <v>771</v>
       </c>
@@ -8889,7 +8985,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="53" spans="1:34" ht="146.25" customHeight="1">
+    <row r="53" spans="1:34" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>785</v>
       </c>
@@ -8969,7 +9065,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="54" spans="1:34" ht="113.25" customHeight="1">
+    <row r="54" spans="1:34" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>801</v>
       </c>
@@ -9043,7 +9139,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:34" ht="389.25">
+    <row r="55" spans="1:34" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>815</v>
       </c>
@@ -9123,7 +9219,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:34" ht="389.25">
+    <row r="56" spans="1:34" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>828</v>
       </c>
@@ -9197,97 +9293,173 @@
         <v>840</v>
       </c>
     </row>
-    <row r="57" spans="1:34">
-      <c r="A57" s="7"/>
+    <row r="57" spans="1:34" ht="360" x14ac:dyDescent="0.2">
+      <c r="A57" s="46" t="s">
+        <v>841</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>842</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>843</v>
+      </c>
+      <c r="D57" s="41" t="s">
+        <v>844</v>
+      </c>
+      <c r="E57" s="42" t="s">
+        <v>845</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>846</v>
+      </c>
+      <c r="H57" s="14">
+        <v>2018</v>
+      </c>
+      <c r="I57" s="43" t="s">
+        <v>847</v>
+      </c>
+      <c r="J57" s="44" t="s">
+        <v>848</v>
+      </c>
+      <c r="K57" s="45" t="s">
+        <v>849</v>
+      </c>
+      <c r="L57" s="45" t="s">
+        <v>849</v>
+      </c>
+      <c r="M57" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="N57" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="O57" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="P57" s="43" t="s">
+        <v>850</v>
+      </c>
+      <c r="Q57" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="R57" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="S57" s="14"/>
+      <c r="T57" s="14" t="s">
+        <v>851</v>
+      </c>
+      <c r="U57" s="14" t="s">
+        <v>852</v>
+      </c>
+      <c r="V57" s="14" t="s">
+        <v>853</v>
+      </c>
+      <c r="W57" s="43" t="s">
+        <v>847</v>
+      </c>
+      <c r="X57" s="14" t="s">
+        <v>854</v>
+      </c>
+      <c r="Y57" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z57" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA57" s="14"/>
     </row>
-    <row r="58" spans="1:34">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
     </row>
-    <row r="59" spans="1:34">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
     </row>
-    <row r="60" spans="1:34">
-      <c r="A60" s="7"/>
+    <row r="60" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:34">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
     </row>
-    <row r="62" spans="1:34">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
     </row>
-    <row r="63" spans="1:34">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
     </row>
-    <row r="64" spans="1:34">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="7"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="7"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="7"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="7"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="7"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="7"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="7"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="7"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="7"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="7"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="7"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="7"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="7"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="7"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="7"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="7"/>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="7"/>
     </row>
   </sheetData>
@@ -9296,12 +9468,24 @@
       <sortCondition ref="A1:A54"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="E57" r:id="rId1" display="https://www.kcl.ac.uk/research/the-sep-md-data-linkage-study" xr:uid="{556AD618-5565-4E79-A417-EB9E2E90EF22}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="b67f489d-6419-4cb0-8238-506a3a8f1300">
@@ -9312,18 +9496,9 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006651BF32B521A046AF14BF632D6B295F" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61ec2f5c856a4823ff415f9801744ae6">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b67f489d-6419-4cb0-8238-506a3a8f1300" xmlns:ns3="0ce01a67-a604-4be1-a4ca-c8b766b5a068" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ab3e104a5ef823f6b61bc0a70e361c14" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006651BF32B521A046AF14BF632D6B295F" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="55423843e2650ade946de227fdfd3c86">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b67f489d-6419-4cb0-8238-506a3a8f1300" xmlns:ns3="0ce01a67-a604-4be1-a4ca-c8b766b5a068" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b15cf6a4d7b0b7ca33e0fb73ec1791d3" ns2:_="" ns3:_="">
     <xsd:import namespace="b67f489d-6419-4cb0-8238-506a3a8f1300"/>
     <xsd:import namespace="0ce01a67-a604-4be1-a4ca-c8b766b5a068"/>
     <xsd:element name="properties">
@@ -9344,6 +9519,7 @@
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -9399,6 +9575,11 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="21" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -9545,13 +9726,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A888961D-86EF-4E4E-8A38-F33DFFA3A067}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C8B3C7C-6A2F-4690-AF82-2D0388819DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C8B3C7C-6A2F-4690-AF82-2D0388819DFC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A888961D-86EF-4E4E-8A38-F33DFFA3A067}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b67f489d-6419-4cb0-8238-506a3a8f1300"/>
+    <ds:schemaRef ds:uri="0ce01a67-a604-4be1-a4ca-c8b766b5a068"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C96B5693-B164-4A92-AE30-985AE2C42908}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B6E6444-F52A-4A7D-907E-4485397AB440}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b67f489d-6419-4cb0-8238-506a3a8f1300"/>
+    <ds:schemaRef ds:uri="0ce01a67-a604-4be1-a4ca-c8b766b5a068"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>